<commit_message>
I have created the script by using my own HDFC account and I have replaced all those values with the dummy values where you can replace your real account details and check the script.
</commit_message>
<xml_diff>
--- a/MavericSystems/data/TC1.xlsx
+++ b/MavericSystems/data/TC1.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\POM\MavericSystems\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11235" windowHeight="4845"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Customer ID</t>
   </si>
@@ -32,10 +28,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>53854092</t>
-  </si>
-  <si>
-    <t>MITHUsri1732$</t>
+    <t>56872904</t>
   </si>
 </sst>
 </file>
@@ -356,7 +349,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -377,7 +372,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>